<commit_message>
good working commit with driggsman page functioning with dp1 table etc
</commit_message>
<xml_diff>
--- a/FileGunBasin/9 August-04 StormBasin/SDDX - ChatGPT Thread Tools Herramientas.xlsx
+++ b/FileGunBasin/9 August-04 StormBasin/SDDX - ChatGPT Thread Tools Herramientas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylecampbell/Documents/repos/localrepo-snefuru4/FileGunBasin/9 August-04 StormBasin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9BF3B7-0314-4747-A6FC-78537B7A09DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566D7582-CC5F-D342-AEA7-DD96FD6818BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19300" xr2:uid="{FC2F1416-21EE-844D-B6FA-128CC66549BB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
   <si>
     <t>https://chatgpt.com/c/68a7137b-772c-8333-8e86-c41cc379bad0</t>
   </si>
@@ -60,6 +60,87 @@
   </si>
   <si>
     <t>Kerberos DB Field Extraction</t>
+  </si>
+  <si>
+    <t>https://chatgpt.com/c/68b2540b-2584-8321-b9c9-9bfaa8ac6050</t>
+  </si>
+  <si>
+    <t>Burnaby Tool</t>
+  </si>
+  <si>
+    <t>please create midjourney prompts for me to use to create logos for my rank and rent websites about duct cleaning they must include no text, be somewhat minimalistic and logo looking. and generally have a transparent bg or can be transitioned easily to a png through a converter tool (from the layout / background of the logo)</t>
+  </si>
+  <si>
+    <t>rank and rent site image logos</t>
+  </si>
+  <si>
+    <t>ann arbor</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>flint</t>
+  </si>
+  <si>
+    <t>jackson</t>
+  </si>
+  <si>
+    <t>tuscaloosa</t>
+  </si>
+  <si>
+    <t>peoria</t>
+  </si>
+  <si>
+    <t>springfield</t>
+  </si>
+  <si>
+    <t>chattanooga</t>
+  </si>
+  <si>
+    <t>charleston</t>
+  </si>
+  <si>
+    <t>augusta</t>
+  </si>
+  <si>
+    <t>ft myers</t>
+  </si>
+  <si>
+    <t>cape coral</t>
+  </si>
+  <si>
+    <t>pembroke pines</t>
+  </si>
+  <si>
+    <t>savannha</t>
+  </si>
+  <si>
+    <t>mi</t>
+  </si>
+  <si>
+    <t>wy</t>
+  </si>
+  <si>
+    <t>al</t>
+  </si>
+  <si>
+    <t>il</t>
+  </si>
+  <si>
+    <t>mo</t>
+  </si>
+  <si>
+    <t>tn</t>
+  </si>
+  <si>
+    <t>sc</t>
+  </si>
+  <si>
+    <t>ga</t>
+  </si>
+  <si>
+    <t>fl</t>
   </si>
 </sst>
 </file>
@@ -142,13 +223,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -484,11 +570,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC59199-8D28-5743-8735-6C342BE5208F}">
-  <dimension ref="E1:E38"/>
+  <dimension ref="A1:AK56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,8 +628,218 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="5:5" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="5:5" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E40" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:37" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I55" t="s">
+        <v>15</v>
+      </c>
+      <c r="J55" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K55" t="s">
+        <v>16</v>
+      </c>
+      <c r="L55" s="7"/>
+      <c r="M55" t="s">
+        <v>17</v>
+      </c>
+      <c r="N55" s="7"/>
+      <c r="O55" t="s">
+        <v>18</v>
+      </c>
+      <c r="P55" s="7"/>
+      <c r="Q55" t="s">
+        <v>19</v>
+      </c>
+      <c r="R55" s="7"/>
+      <c r="S55" t="s">
+        <v>20</v>
+      </c>
+      <c r="T55" s="7"/>
+      <c r="U55" t="s">
+        <v>21</v>
+      </c>
+      <c r="V55" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W55" t="s">
+        <v>21</v>
+      </c>
+      <c r="X55" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z55" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB55" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC55" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD55" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE55" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF55" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG55" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH55" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI55" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ55" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK55" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A56" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I56" t="s">
+        <v>27</v>
+      </c>
+      <c r="J56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K56" t="s">
+        <v>28</v>
+      </c>
+      <c r="L56" s="7"/>
+      <c r="M56" t="s">
+        <v>29</v>
+      </c>
+      <c r="N56" s="7"/>
+      <c r="O56" t="s">
+        <v>30</v>
+      </c>
+      <c r="P56" s="7"/>
+      <c r="Q56" t="s">
+        <v>31</v>
+      </c>
+      <c r="R56" s="7"/>
+      <c r="S56" t="s">
+        <v>32</v>
+      </c>
+      <c r="T56" s="7"/>
+      <c r="U56" t="s">
+        <v>33</v>
+      </c>
+      <c r="V56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W56" t="s">
+        <v>33</v>
+      </c>
+      <c r="X56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC56" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE56" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG56" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI56" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK56" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E26" r:id="rId1" xr:uid="{857A59AE-994A-EB4E-B220-0CFF303AA7B2}"/>

</xml_diff>